<commit_message>
add csv for basic 20q
</commit_message>
<xml_diff>
--- a/neuralnets/practical/initialconcepts.xlsx
+++ b/neuralnets/practical/initialconcepts.xlsx
@@ -162,10 +162,10 @@
     <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -177,7 +177,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -185,7 +185,7 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -193,7 +193,7 @@
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -201,7 +201,7 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -209,7 +209,7 @@
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -217,7 +217,7 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -225,7 +225,7 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -233,12 +233,12 @@
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
better explain basic 20q concepts in spreadsheet
</commit_message>
<xml_diff>
--- a/neuralnets/practical/initialconcepts.xlsx
+++ b/neuralnets/practical/initialconcepts.xlsx
@@ -29,7 +29,7 @@
     <t>phone</t>
   </si>
   <si>
-    <t>do you use it with your hand</t>
+    <t>is it electronic</t>
   </si>
   <si>
     <t>window</t>
@@ -80,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,13 +160,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -174,71 +175,95 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>